<commit_message>
Fully modularised and made it work
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Softeng 762\Project\softeng762\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Coding Stuff\SE762\softeng762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A0514A-136F-4A10-BA67-CD50607D7B50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37442E4B-4C87-4026-BDD0-C14CB9236FAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{8DA7EBCB-5E4B-4457-A20E-ACC4E9E1C078}"/>
+    <workbookView xWindow="0" yWindow="4365" windowWidth="28800" windowHeight="15435" xr2:uid="{8DA7EBCB-5E4B-4457-A20E-ACC4E9E1C078}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -484,10 +484,10 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G3">
-        <v>261940721</v>
+        <v>184846458</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cleared the sheet before adding in data
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Coding Stuff\SE762\softeng762\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Softeng 762\Project\softeng762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37442E4B-4C87-4026-BDD0-C14CB9236FAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA5C057-5E75-4DD2-B052-CE388231D39F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4365" windowWidth="28800" windowHeight="15435" xr2:uid="{8DA7EBCB-5E4B-4457-A20E-ACC4E9E1C078}"/>
+    <workbookView xWindow="-28800" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{8DA7EBCB-5E4B-4457-A20E-ACC4E9E1C078}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,38 +414,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F3A383-65A2-4C9E-8C3B-0E83440D0644}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -467,9 +468,9 @@
         <v>261940721</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -484,13 +485,13 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3">
-        <v>184846458</v>
+        <v>261940721</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -513,7 +514,7 @@
         <v>184846458</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -535,6 +536,9 @@
       <c r="G5">
         <v>184846458</v>
       </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed modules to only use 1 global path. Added checks for zip files and csv files
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Softeng 762\Project\softeng762\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Coding Stuff\SE762\softeng762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA5C057-5E75-4DD2-B052-CE388231D39F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AF531F-DCA8-4655-A122-4ABCE60B4252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{8DA7EBCB-5E4B-4457-A20E-ACC4E9E1C078}"/>
+    <workbookView xWindow="0" yWindow="4365" windowWidth="28800" windowHeight="15435" xr2:uid="{8DA7EBCB-5E4B-4457-A20E-ACC4E9E1C078}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Sortable name</t>
   </si>
@@ -414,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F3A383-65A2-4C9E-8C3B-0E83440D0644}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -422,7 +422,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -445,7 +445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -456,21 +456,27 @@
         <v>8</v>
       </c>
       <c r="D2" s="1">
-        <v>44112</v>
+        <v>44115</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>261940721</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -479,65 +485,31 @@
         <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>44112</v>
+        <v>44121</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3">
-        <v>261940721</v>
+      <c r="F3">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3">
+        <v>184846458</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44112</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4">
-        <v>184846458</v>
-      </c>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44112</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5">
-        <v>184846458</v>
-      </c>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" s="2"/>
     </row>
   </sheetData>

</xml_diff>